<commit_message>
function update suspense fifa
update suspense for fifa criteria when teams are level, should do the same for uefa criteria.
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/wc/goals_wc_fifa.xlsx
+++ b/data/out/wiki/men/fifa/wc/goals_wc_fifa.xlsx
@@ -683,7 +683,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Hungary', 'France']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Hungary', 'France']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="AR3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -995,7 +995,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Hungary', 'France']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -1108,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Hungary', 'France']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="AR5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Hungary', 'France']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="AR6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Hungary', 'France']</t>
+          <t>['Hungary', 'France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1582,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="AR7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1613,7 +1613,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="AR9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="AR10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="AR12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="AR13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -2670,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="AR14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Argentina', 'Italy']</t>
+          <t>['Argentina', 'Bulgaria', 'Italy']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['Belgium', 'Mexico', 'Paraguay']</t>
+          <t>['Mexico', 'Belgium', 'Paraguay']</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -3126,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="AR17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="AR18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -3442,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="AR19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -3600,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="AR20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -3758,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="AR21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -3789,7 +3789,7 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['Portugal', 'Morocco', 'Poland']</t>
+          <t>['Morocco', 'Portugal', 'Poland']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['Portugal', 'England', 'Poland']</t>
+          <t>['Portugal', 'Poland', 'England']</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -4056,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="AR23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['Portugal', 'England', 'Morocco']</t>
+          <t>['Morocco', 'Portugal', 'England']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -4214,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="AR24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -4259,7 +4259,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Morocco', 'Poland', 'England']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -4417,7 +4417,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Morocco', 'Poland', 'England']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -4530,7 +4530,7 @@
         <v>0</v>
       </c>
       <c r="AR26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Morocco', 'Poland', 'England']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -4688,7 +4688,7 @@
         <v>0</v>
       </c>
       <c r="AR27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Morocco', 'Poland', 'England']</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -4846,7 +4846,7 @@
         <v>0</v>
       </c>
       <c r="AR28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -4891,7 +4891,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Morocco', 'Poland', 'England']</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -5035,7 +5035,7 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
-          <t>['Brazil', 'Northern Ireland', 'Spain']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['Brazil', 'Algeria', 'Spain']</t>
+          <t>['Spain', 'Algeria', 'Brazil']</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -5302,7 +5302,7 @@
         <v>0</v>
       </c>
       <c r="AR31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>['Brazil', 'Northern Ireland', 'Spain']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -5460,7 +5460,7 @@
         <v>0</v>
       </c>
       <c r="AR32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -5505,7 +5505,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['Brazil', 'Algeria', 'Spain']</t>
+          <t>['Spain', 'Algeria', 'Brazil']</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -5618,7 +5618,7 @@
         <v>1</v>
       </c>
       <c r="AR33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>['Brazil', 'Northern Ireland', 'Spain']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -5776,7 +5776,7 @@
         <v>0</v>
       </c>
       <c r="AR34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>['Brazil', 'Northern Ireland', 'Spain']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -5934,7 +5934,7 @@
         <v>0</v>
       </c>
       <c r="AR35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -5979,7 +5979,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>['Brazil', 'Northern Ireland', 'Spain']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -6092,7 +6092,7 @@
         <v>0</v>
       </c>
       <c r="AR36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -6123,7 +6123,7 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t>['West Germany', 'Denmark', 'Uruguay']</t>
+          <t>['Uruguay', 'Denmark', 'West Germany']</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -6277,7 +6277,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>['West Germany', 'Denmark', 'Uruguay']</t>
+          <t>['Uruguay', 'Denmark', 'West Germany']</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -6390,7 +6390,7 @@
         <v>1</v>
       </c>
       <c r="AR38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -6435,7 +6435,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>['West Germany', 'Denmark', 'Uruguay']</t>
+          <t>['Uruguay', 'Denmark', 'West Germany']</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -6548,7 +6548,7 @@
         <v>1</v>
       </c>
       <c r="AR39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -6579,7 +6579,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>['Argentina', 'Cameroon', 'Romania']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -6733,7 +6733,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>['Argentina', 'Cameroon', 'Romania']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -6846,7 +6846,7 @@
         <v>0</v>
       </c>
       <c r="AR41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -6891,7 +6891,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>['Argentina', 'Cameroon', 'Romania']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -7004,7 +7004,7 @@
         <v>0</v>
       </c>
       <c r="AR42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -7049,7 +7049,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>['Argentina', 'Cameroon', 'Romania']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -7162,7 +7162,7 @@
         <v>0</v>
       </c>
       <c r="AR43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -7365,7 +7365,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Argentina', 'Cameroon']</t>
+          <t>['Argentina', 'Cameroon', 'Soviet Union']</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -7478,7 +7478,7 @@
         <v>0</v>
       </c>
       <c r="AR45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>['Argentina', 'Cameroon', 'Romania']</t>
+          <t>['Romania', 'Argentina', 'Cameroon']</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -7636,7 +7636,7 @@
         <v>0</v>
       </c>
       <c r="AR46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -7667,7 +7667,7 @@
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -7821,7 +7821,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -7934,7 +7934,7 @@
         <v>0</v>
       </c>
       <c r="AR48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -7979,7 +7979,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -8092,7 +8092,7 @@
         <v>0</v>
       </c>
       <c r="AR49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -8137,7 +8137,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -8250,7 +8250,7 @@
         <v>0</v>
       </c>
       <c r="AR50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -8295,7 +8295,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -8408,7 +8408,7 @@
         <v>0</v>
       </c>
       <c r="AR51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -8453,7 +8453,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -8566,7 +8566,7 @@
         <v>0</v>
       </c>
       <c r="AR52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -8611,7 +8611,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -8724,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="AR53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -8769,7 +8769,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['West Germany', 'Yugoslavia', 'Colombia']</t>
+          <t>['Colombia', 'Yugoslavia', 'West Germany']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -8913,7 +8913,7 @@
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['Czechoslovakia', 'Austria', 'Italy']</t>
+          <t>['Italy', 'Austria', 'Czechoslovakia']</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -9180,7 +9180,7 @@
         <v>0</v>
       </c>
       <c r="AR56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -9338,7 +9338,7 @@
         <v>0</v>
       </c>
       <c r="AR57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -9496,7 +9496,7 @@
         <v>1</v>
       </c>
       <c r="AR58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -9654,7 +9654,7 @@
         <v>1</v>
       </c>
       <c r="AR59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -9812,7 +9812,7 @@
         <v>0</v>
       </c>
       <c r="AR60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -9843,7 +9843,7 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -9997,7 +9997,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['Brazil', 'Scotland', 'Sweden']</t>
+          <t>['Scotland', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -10110,7 +10110,7 @@
         <v>1</v>
       </c>
       <c r="AR62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -10155,7 +10155,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -10268,7 +10268,7 @@
         <v>0</v>
       </c>
       <c r="AR63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -10313,7 +10313,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -10471,7 +10471,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -10584,7 +10584,7 @@
         <v>0</v>
       </c>
       <c r="AR65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -10615,7 +10615,7 @@
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Belgium', 'Spain', 'Uruguay']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -10769,7 +10769,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Belgium', 'Spain', 'Uruguay']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -10882,7 +10882,7 @@
         <v>0</v>
       </c>
       <c r="AR67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -10927,7 +10927,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Belgium', 'Spain', 'Uruguay']</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -11040,7 +11040,7 @@
         <v>0</v>
       </c>
       <c r="AR68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -11085,7 +11085,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Belgium', 'Spain', 'Uruguay']</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -11198,7 +11198,7 @@
         <v>0</v>
       </c>
       <c r="AR69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -11243,7 +11243,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>['Belgium', 'Uruguay', 'Spain']</t>
+          <t>['Belgium', 'Spain', 'Uruguay']</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -11356,7 +11356,7 @@
         <v>1</v>
       </c>
       <c r="AR70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -11541,7 +11541,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>['England', 'Egypt', 'Netherlands']</t>
+          <t>['Egypt', 'England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -11654,7 +11654,7 @@
         <v>0</v>
       </c>
       <c r="AR72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -11699,7 +11699,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>['England', 'Egypt', 'Netherlands']</t>
+          <t>['Egypt', 'England', 'Netherlands']</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -11812,7 +11812,7 @@
         <v>1</v>
       </c>
       <c r="AR73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -12001,7 +12001,7 @@
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
         <is>
-          <t>['United States', 'Switzerland', 'Romania']</t>
+          <t>['Romania', 'United States', 'Switzerland']</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -12155,7 +12155,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>['United States', 'Switzerland', 'Romania']</t>
+          <t>['Romania', 'United States', 'Switzerland']</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -12268,7 +12268,7 @@
         <v>0</v>
       </c>
       <c r="AR76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -12313,7 +12313,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>['United States', 'Switzerland', 'Romania']</t>
+          <t>['Romania', 'United States', 'Switzerland']</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -12426,7 +12426,7 @@
         <v>0</v>
       </c>
       <c r="AR77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -12471,7 +12471,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>['United States', 'Switzerland', 'Romania']</t>
+          <t>['Romania', 'United States', 'Switzerland']</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -12584,7 +12584,7 @@
         <v>0</v>
       </c>
       <c r="AR78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -12615,7 +12615,7 @@
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -12769,7 +12769,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -12882,7 +12882,7 @@
         <v>0</v>
       </c>
       <c r="AR80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -12927,7 +12927,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -13040,7 +13040,7 @@
         <v>0</v>
       </c>
       <c r="AR81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -13085,7 +13085,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -13198,7 +13198,7 @@
         <v>0</v>
       </c>
       <c r="AR82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -13243,7 +13243,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -13356,7 +13356,7 @@
         <v>0</v>
       </c>
       <c r="AR83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -13401,7 +13401,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -13514,7 +13514,7 @@
         <v>0</v>
       </c>
       <c r="AR84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -13559,7 +13559,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -13672,7 +13672,7 @@
         <v>0</v>
       </c>
       <c r="AR85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -13717,7 +13717,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -13875,7 +13875,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -13988,7 +13988,7 @@
         <v>0</v>
       </c>
       <c r="AR87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -14033,7 +14033,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>['South Korea', 'Germany', 'Spain']</t>
+          <t>['South Korea', 'Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -14146,7 +14146,7 @@
         <v>0</v>
       </c>
       <c r="AR88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -14331,7 +14331,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>['Ireland', 'Italy', 'Norway']</t>
+          <t>['Ireland', 'Norway', 'Italy']</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -14444,7 +14444,7 @@
         <v>0</v>
       </c>
       <c r="AR90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -14602,7 +14602,7 @@
         <v>0</v>
       </c>
       <c r="AR91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -14633,7 +14633,7 @@
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr">
         <is>
-          <t>['Brazil', 'Cameroon', 'Sweden']</t>
+          <t>['Brazil', 'Sweden', 'Cameroon']</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -14787,7 +14787,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -14900,7 +14900,7 @@
         <v>0</v>
       </c>
       <c r="AR93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -14945,7 +14945,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
@@ -15058,7 +15058,7 @@
         <v>0</v>
       </c>
       <c r="AR94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -15103,7 +15103,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -15216,7 +15216,7 @@
         <v>0</v>
       </c>
       <c r="AR95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -15261,7 +15261,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -15374,7 +15374,7 @@
         <v>0</v>
       </c>
       <c r="AR96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -15419,7 +15419,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -15532,7 +15532,7 @@
         <v>0</v>
       </c>
       <c r="AR97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -15577,7 +15577,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
@@ -15690,7 +15690,7 @@
         <v>0</v>
       </c>
       <c r="AR98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -15735,7 +15735,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
@@ -15893,7 +15893,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
@@ -16006,7 +16006,7 @@
         <v>1</v>
       </c>
       <c r="AR100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -16051,7 +16051,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>['Brazil', 'Sweden', 'Russia']</t>
+          <t>['Russia', 'Brazil', 'Sweden']</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -16164,7 +16164,7 @@
         <v>1</v>
       </c>
       <c r="AR101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -16195,7 +16195,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands', 'Saudi Arabia']</t>
+          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -16349,7 +16349,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands', 'Saudi Arabia']</t>
+          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -16462,7 +16462,7 @@
         <v>1</v>
       </c>
       <c r="AR103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -16507,7 +16507,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands', 'Saudi Arabia']</t>
+          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -16620,7 +16620,7 @@
         <v>0</v>
       </c>
       <c r="AR104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -16665,7 +16665,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands', 'Saudi Arabia']</t>
+          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -16823,7 +16823,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands', 'Saudi Arabia']</t>
+          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -16936,7 +16936,7 @@
         <v>0</v>
       </c>
       <c r="AR106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -16967,7 +16967,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
+          <t>['Argentina', 'Nigeria', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -17121,7 +17121,7 @@
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
+          <t>['Argentina', 'Nigeria', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
@@ -17234,7 +17234,7 @@
         <v>0</v>
       </c>
       <c r="AR108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -17279,7 +17279,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
+          <t>['Argentina', 'Nigeria', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -17392,7 +17392,7 @@
         <v>0</v>
       </c>
       <c r="AR109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -17437,7 +17437,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Bulgaria', 'Argentina']</t>
+          <t>['Bulgaria', 'Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -17550,7 +17550,7 @@
         <v>0</v>
       </c>
       <c r="AR110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -17595,7 +17595,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Bulgaria', 'Argentina']</t>
+          <t>['Bulgaria', 'Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -17708,7 +17708,7 @@
         <v>0</v>
       </c>
       <c r="AR111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -18006,7 +18006,7 @@
         <v>0</v>
       </c>
       <c r="AR113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -18164,7 +18164,7 @@
         <v>0</v>
       </c>
       <c r="AR114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -18322,7 +18322,7 @@
         <v>0</v>
       </c>
       <c r="AR115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -18480,7 +18480,7 @@
         <v>0</v>
       </c>
       <c r="AR116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -18638,7 +18638,7 @@
         <v>0</v>
       </c>
       <c r="AR117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
@@ -18669,7 +18669,7 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr">
         <is>
-          <t>['Brazil', 'Norway']</t>
+          <t>['Norway', 'Brazil']</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
@@ -18823,7 +18823,7 @@
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K119" t="inlineStr">
@@ -18936,7 +18936,7 @@
         <v>0</v>
       </c>
       <c r="AR119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -18981,7 +18981,7 @@
       </c>
       <c r="J120" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K120" t="inlineStr">
@@ -19094,7 +19094,7 @@
         <v>0</v>
       </c>
       <c r="AR120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -19139,7 +19139,7 @@
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K121" t="inlineStr">
@@ -19252,7 +19252,7 @@
         <v>0</v>
       </c>
       <c r="AR121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -19297,7 +19297,7 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K122" t="inlineStr">
@@ -19455,7 +19455,7 @@
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K123" t="inlineStr">
@@ -19568,7 +19568,7 @@
         <v>0</v>
       </c>
       <c r="AR123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
@@ -19613,7 +19613,7 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>['Brazil', 'Norway']</t>
+          <t>['Norway', 'Brazil']</t>
         </is>
       </c>
       <c r="K124" t="inlineStr">
@@ -19726,7 +19726,7 @@
         <v>0</v>
       </c>
       <c r="AR124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -20024,7 +20024,7 @@
         <v>0</v>
       </c>
       <c r="AR126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -20182,7 +20182,7 @@
         <v>0</v>
       </c>
       <c r="AR127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -20340,7 +20340,7 @@
         <v>0</v>
       </c>
       <c r="AR128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -20498,7 +20498,7 @@
         <v>0</v>
       </c>
       <c r="AR129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -20656,7 +20656,7 @@
         <v>0</v>
       </c>
       <c r="AR130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -20814,7 +20814,7 @@
         <v>0</v>
       </c>
       <c r="AR131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -21270,7 +21270,7 @@
         <v>0</v>
       </c>
       <c r="AR134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -21428,7 +21428,7 @@
         <v>0</v>
       </c>
       <c r="AR135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -21473,7 +21473,7 @@
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Spain']</t>
+          <t>['Spain', 'Nigeria']</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
@@ -21631,7 +21631,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Spain']</t>
+          <t>['Spain', 'Nigeria']</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
@@ -21789,7 +21789,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Spain']</t>
+          <t>['Spain', 'Nigeria']</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
@@ -21902,7 +21902,7 @@
         <v>0</v>
       </c>
       <c r="AR138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -22060,7 +22060,7 @@
         <v>0</v>
       </c>
       <c r="AR139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -22376,7 +22376,7 @@
         <v>0</v>
       </c>
       <c r="AR141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -22534,7 +22534,7 @@
         <v>0</v>
       </c>
       <c r="AR142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -22692,7 +22692,7 @@
         <v>0</v>
       </c>
       <c r="AR143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -23148,7 +23148,7 @@
         <v>0</v>
       </c>
       <c r="AR146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -23306,7 +23306,7 @@
         <v>0</v>
       </c>
       <c r="AR147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -23464,7 +23464,7 @@
         <v>0</v>
       </c>
       <c r="AR148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -23780,7 +23780,7 @@
         <v>0</v>
       </c>
       <c r="AR150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -23938,7 +23938,7 @@
         <v>0</v>
       </c>
       <c r="AR151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -23969,7 +23969,7 @@
       <c r="I152" t="inlineStr"/>
       <c r="J152" t="inlineStr">
         <is>
-          <t>['Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Germany']</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -24123,7 +24123,7 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>['Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Germany']</t>
         </is>
       </c>
       <c r="K153" t="inlineStr">
@@ -24236,7 +24236,7 @@
         <v>1</v>
       </c>
       <c r="AR153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -24281,7 +24281,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>['Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Germany']</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -24394,7 +24394,7 @@
         <v>0</v>
       </c>
       <c r="AR154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -24439,7 +24439,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>['Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Germany']</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -24552,7 +24552,7 @@
         <v>0</v>
       </c>
       <c r="AR155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
@@ -24850,7 +24850,7 @@
         <v>0</v>
       </c>
       <c r="AR157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -25008,7 +25008,7 @@
         <v>0</v>
       </c>
       <c r="AR158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -25166,7 +25166,7 @@
         <v>0</v>
       </c>
       <c r="AR159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -25324,7 +25324,7 @@
         <v>0</v>
       </c>
       <c r="AR160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -25355,7 +25355,7 @@
       <c r="I161" t="inlineStr"/>
       <c r="J161" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
@@ -25622,7 +25622,7 @@
         <v>1</v>
       </c>
       <c r="AR162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -25667,7 +25667,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -25780,7 +25780,7 @@
         <v>0</v>
       </c>
       <c r="AR163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -25825,7 +25825,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -25938,7 +25938,7 @@
         <v>0</v>
       </c>
       <c r="AR164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -25983,7 +25983,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -26096,7 +26096,7 @@
         <v>1</v>
       </c>
       <c r="AR165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -26127,7 +26127,7 @@
       <c r="I166" t="inlineStr"/>
       <c r="J166" t="inlineStr">
         <is>
-          <t>['Senegal', 'Denmark']</t>
+          <t>['Denmark', 'Senegal']</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
@@ -26394,7 +26394,7 @@
         <v>1</v>
       </c>
       <c r="AR167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -26439,7 +26439,7 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>['Senegal', 'Denmark']</t>
+          <t>['Denmark', 'Senegal']</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">
@@ -26552,7 +26552,7 @@
         <v>1</v>
       </c>
       <c r="AR168" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -26710,7 +26710,7 @@
         <v>1</v>
       </c>
       <c r="AR169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -26868,7 +26868,7 @@
         <v>1</v>
       </c>
       <c r="AR170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
@@ -27026,7 +27026,7 @@
         <v>1</v>
       </c>
       <c r="AR171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -27184,7 +27184,7 @@
         <v>0</v>
       </c>
       <c r="AR172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -27229,7 +27229,7 @@
       </c>
       <c r="J173" t="inlineStr">
         <is>
-          <t>['Senegal', 'Denmark']</t>
+          <t>['Denmark', 'Senegal']</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
@@ -27387,7 +27387,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>['Senegal', 'Denmark']</t>
+          <t>['Denmark', 'Senegal']</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
@@ -27531,7 +27531,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>['Germany', 'Cameroon']</t>
+          <t>['Cameroon', 'Germany']</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -27685,7 +27685,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -27798,7 +27798,7 @@
         <v>1</v>
       </c>
       <c r="AR176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -27843,7 +27843,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -27956,7 +27956,7 @@
         <v>0</v>
       </c>
       <c r="AR177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178">
@@ -28001,7 +28001,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -28114,7 +28114,7 @@
         <v>0</v>
       </c>
       <c r="AR178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -28159,7 +28159,7 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -28272,7 +28272,7 @@
         <v>0</v>
       </c>
       <c r="AR179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -28317,7 +28317,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Germany', 'Ireland']</t>
+          <t>['Ireland', 'Germany']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -28430,7 +28430,7 @@
         <v>0</v>
       </c>
       <c r="AR180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
@@ -28728,7 +28728,7 @@
         <v>0</v>
       </c>
       <c r="AR182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -28886,7 +28886,7 @@
         <v>0</v>
       </c>
       <c r="AR183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -28917,7 +28917,7 @@
       <c r="I184" t="inlineStr"/>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -29071,7 +29071,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -29184,7 +29184,7 @@
         <v>0</v>
       </c>
       <c r="AR185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -29229,7 +29229,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -29342,7 +29342,7 @@
         <v>0</v>
       </c>
       <c r="AR186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -29387,7 +29387,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
@@ -29500,7 +29500,7 @@
         <v>0</v>
       </c>
       <c r="AR187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">
@@ -29545,7 +29545,7 @@
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -29658,7 +29658,7 @@
         <v>0</v>
       </c>
       <c r="AR188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -29703,7 +29703,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -29816,7 +29816,7 @@
         <v>0</v>
       </c>
       <c r="AR189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -29861,7 +29861,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -29974,7 +29974,7 @@
         <v>0</v>
       </c>
       <c r="AR190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -30019,7 +30019,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -30177,7 +30177,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -30335,7 +30335,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Spain']</t>
+          <t>['Spain', 'Paraguay']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -30448,7 +30448,7 @@
         <v>0</v>
       </c>
       <c r="AR193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -30479,7 +30479,7 @@
       <c r="I194" t="inlineStr"/>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Brazil']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -30633,7 +30633,7 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Brazil']</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -30746,7 +30746,7 @@
         <v>0</v>
       </c>
       <c r="AR195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -30791,7 +30791,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Brazil']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -30904,7 +30904,7 @@
         <v>0</v>
       </c>
       <c r="AR196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -31062,7 +31062,7 @@
         <v>0</v>
       </c>
       <c r="AR197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
@@ -31220,7 +31220,7 @@
         <v>0</v>
       </c>
       <c r="AR198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
@@ -31378,7 +31378,7 @@
         <v>0</v>
       </c>
       <c r="AR199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -31581,7 +31581,7 @@
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Brazil']</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -32010,7 +32010,7 @@
         <v>0</v>
       </c>
       <c r="AR203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -32168,7 +32168,7 @@
         <v>0</v>
       </c>
       <c r="AR204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
@@ -32466,7 +32466,7 @@
         <v>0</v>
       </c>
       <c r="AR206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -32624,7 +32624,7 @@
         <v>0</v>
       </c>
       <c r="AR207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208">
@@ -32782,7 +32782,7 @@
         <v>0</v>
       </c>
       <c r="AR208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -32813,7 +32813,7 @@
       <c r="I209" t="inlineStr"/>
       <c r="J209" t="inlineStr">
         <is>
-          <t>['Russia', 'Japan']</t>
+          <t>['Japan', 'Russia']</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -33080,7 +33080,7 @@
         <v>0</v>
       </c>
       <c r="AR210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
@@ -33125,7 +33125,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -33238,7 +33238,7 @@
         <v>1</v>
       </c>
       <c r="AR211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
@@ -33283,7 +33283,7 @@
       </c>
       <c r="J212" t="inlineStr">
         <is>
-          <t>['Russia', 'Japan']</t>
+          <t>['Japan', 'Russia']</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
@@ -33441,7 +33441,7 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>['Russia', 'Japan']</t>
+          <t>['Japan', 'Russia']</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
@@ -33599,7 +33599,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -33712,7 +33712,7 @@
         <v>1</v>
       </c>
       <c r="AR214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -33757,7 +33757,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -33870,7 +33870,7 @@
         <v>1</v>
       </c>
       <c r="AR215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216">
@@ -33915,7 +33915,7 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -34213,7 +34213,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['Portugal', 'South Korea']</t>
+          <t>['South Korea', 'Portugal']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -34326,7 +34326,7 @@
         <v>0</v>
       </c>
       <c r="AR218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -34371,7 +34371,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['Portugal', 'South Korea']</t>
+          <t>['South Korea', 'Portugal']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -34484,7 +34484,7 @@
         <v>0</v>
       </c>
       <c r="AR219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -34529,7 +34529,7 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>['Portugal', 'South Korea']</t>
+          <t>['South Korea', 'Portugal']</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -34642,7 +34642,7 @@
         <v>0</v>
       </c>
       <c r="AR220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -34958,7 +34958,7 @@
         <v>0</v>
       </c>
       <c r="AR222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
@@ -34989,7 +34989,7 @@
       <c r="I223" t="inlineStr"/>
       <c r="J223" t="inlineStr">
         <is>
-          <t>['Germany', 'Ecuador']</t>
+          <t>['Ecuador', 'Germany']</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
@@ -35143,7 +35143,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>['Germany', 'Ecuador']</t>
+          <t>['Ecuador', 'Germany']</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -35256,7 +35256,7 @@
         <v>0</v>
       </c>
       <c r="AR224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225">
@@ -35301,7 +35301,7 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>['Germany', 'Ecuador']</t>
+          <t>['Ecuador', 'Germany']</t>
         </is>
       </c>
       <c r="K225" t="inlineStr">
@@ -35414,7 +35414,7 @@
         <v>0</v>
       </c>
       <c r="AR225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -35459,7 +35459,7 @@
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>['Germany', 'Ecuador']</t>
+          <t>['Ecuador', 'Germany']</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -35572,7 +35572,7 @@
         <v>0</v>
       </c>
       <c r="AR226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227">
@@ -35617,7 +35617,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>['Germany', 'Ecuador']</t>
+          <t>['Ecuador', 'Germany']</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -35730,7 +35730,7 @@
         <v>0</v>
       </c>
       <c r="AR227" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228">
@@ -35775,7 +35775,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Germany', 'Ecuador']</t>
+          <t>['Ecuador', 'Germany']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -35888,7 +35888,7 @@
         <v>0</v>
       </c>
       <c r="AR228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -35933,7 +35933,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Germany', 'Ecuador']</t>
+          <t>['Ecuador', 'Germany']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -36046,7 +36046,7 @@
         <v>0</v>
       </c>
       <c r="AR229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -36344,7 +36344,7 @@
         <v>0</v>
       </c>
       <c r="AR231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232">
@@ -36502,7 +36502,7 @@
         <v>0</v>
       </c>
       <c r="AR232" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233">
@@ -36660,7 +36660,7 @@
         <v>0</v>
       </c>
       <c r="AR233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234">
@@ -36818,7 +36818,7 @@
         <v>0</v>
       </c>
       <c r="AR234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">
@@ -36976,7 +36976,7 @@
         <v>0</v>
       </c>
       <c r="AR235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236">
@@ -37134,7 +37134,7 @@
         <v>0</v>
       </c>
       <c r="AR236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -37165,7 +37165,7 @@
       <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Portugal', 'Mexico']</t>
+          <t>['Mexico', 'Portugal']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -37319,7 +37319,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Portugal', 'Mexico']</t>
+          <t>['Mexico', 'Portugal']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -37432,7 +37432,7 @@
         <v>0</v>
       </c>
       <c r="AR238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239">
@@ -37477,7 +37477,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Portugal', 'Mexico']</t>
+          <t>['Mexico', 'Portugal']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -37590,7 +37590,7 @@
         <v>0</v>
       </c>
       <c r="AR239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240">
@@ -37635,7 +37635,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>['Portugal', 'Mexico']</t>
+          <t>['Mexico', 'Portugal']</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -37748,7 +37748,7 @@
         <v>0</v>
       </c>
       <c r="AR240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241">
@@ -37793,7 +37793,7 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>['Portugal', 'Mexico']</t>
+          <t>['Mexico', 'Portugal']</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
@@ -37906,7 +37906,7 @@
         <v>0</v>
       </c>
       <c r="AR241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242">
@@ -37951,7 +37951,7 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>['Portugal', 'Mexico']</t>
+          <t>['Mexico', 'Portugal']</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
@@ -38064,7 +38064,7 @@
         <v>0</v>
       </c>
       <c r="AR242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243">
@@ -38362,7 +38362,7 @@
         <v>0</v>
       </c>
       <c r="AR244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -38520,7 +38520,7 @@
         <v>0</v>
       </c>
       <c r="AR245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246">
@@ -38678,7 +38678,7 @@
         <v>0</v>
       </c>
       <c r="AR246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247">
@@ -38836,7 +38836,7 @@
         <v>0</v>
       </c>
       <c r="AR247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="248">
@@ -38994,7 +38994,7 @@
         <v>0</v>
       </c>
       <c r="AR248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249">
@@ -39292,7 +39292,7 @@
         <v>1</v>
       </c>
       <c r="AR250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
@@ -39450,7 +39450,7 @@
         <v>0</v>
       </c>
       <c r="AR251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252">
@@ -39766,7 +39766,7 @@
         <v>0</v>
       </c>
       <c r="AR253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">
@@ -39924,7 +39924,7 @@
         <v>0</v>
       </c>
       <c r="AR254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="255">
@@ -40222,7 +40222,7 @@
         <v>1</v>
       </c>
       <c r="AR256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
@@ -40380,7 +40380,7 @@
         <v>0</v>
       </c>
       <c r="AR257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258">
@@ -40538,7 +40538,7 @@
         <v>0</v>
       </c>
       <c r="AR258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259">
@@ -40854,7 +40854,7 @@
         <v>1</v>
       </c>
       <c r="AR260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261">
@@ -41784,7 +41784,7 @@
         <v>1</v>
       </c>
       <c r="AR266" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -41942,7 +41942,7 @@
         <v>1</v>
       </c>
       <c r="AR267" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268">
@@ -42240,7 +42240,7 @@
         <v>0</v>
       </c>
       <c r="AR269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270">
@@ -42398,7 +42398,7 @@
         <v>0</v>
       </c>
       <c r="AR270" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271">
@@ -42556,7 +42556,7 @@
         <v>0</v>
       </c>
       <c r="AR271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272">
@@ -42714,7 +42714,7 @@
         <v>0</v>
       </c>
       <c r="AR272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">
@@ -43012,7 +43012,7 @@
         <v>0</v>
       </c>
       <c r="AR274" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275">
@@ -43170,7 +43170,7 @@
         <v>0</v>
       </c>
       <c r="AR275" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276">
@@ -43328,7 +43328,7 @@
         <v>0</v>
       </c>
       <c r="AR276" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277">
@@ -43486,7 +43486,7 @@
         <v>0</v>
       </c>
       <c r="AR277" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="278">
@@ -43671,7 +43671,7 @@
       </c>
       <c r="J279" t="inlineStr">
         <is>
-          <t>['Greece', 'Argentina']</t>
+          <t>['Argentina', 'Greece']</t>
         </is>
       </c>
       <c r="K279" t="inlineStr">
@@ -43784,7 +43784,7 @@
         <v>0</v>
       </c>
       <c r="AR279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280">
@@ -43942,7 +43942,7 @@
         <v>0</v>
       </c>
       <c r="AR280" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281">
@@ -44100,7 +44100,7 @@
         <v>0</v>
       </c>
       <c r="AR281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282">
@@ -44258,7 +44258,7 @@
         <v>0</v>
       </c>
       <c r="AR282" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283">
@@ -44416,7 +44416,7 @@
         <v>0</v>
       </c>
       <c r="AR283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284">
@@ -44574,7 +44574,7 @@
         <v>0</v>
       </c>
       <c r="AR284" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285">
@@ -44759,7 +44759,7 @@
       </c>
       <c r="J286" t="inlineStr">
         <is>
-          <t>['England', 'Slovenia']</t>
+          <t>['Slovenia', 'England']</t>
         </is>
       </c>
       <c r="K286" t="inlineStr">
@@ -44872,7 +44872,7 @@
         <v>0</v>
       </c>
       <c r="AR286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287">
@@ -45030,7 +45030,7 @@
         <v>1</v>
       </c>
       <c r="AR287" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288">
@@ -45328,7 +45328,7 @@
         <v>0</v>
       </c>
       <c r="AR289" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290">
@@ -45486,7 +45486,7 @@
         <v>0</v>
       </c>
       <c r="AR290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291">
@@ -45644,7 +45644,7 @@
         <v>0</v>
       </c>
       <c r="AR291" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292">
@@ -45802,7 +45802,7 @@
         <v>0</v>
       </c>
       <c r="AR292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293">
@@ -45833,7 +45833,7 @@
       <c r="I293" t="inlineStr"/>
       <c r="J293" t="inlineStr">
         <is>
-          <t>['Italy', 'Paraguay']</t>
+          <t>['Paraguay', 'Italy']</t>
         </is>
       </c>
       <c r="K293" t="inlineStr">
@@ -46100,7 +46100,7 @@
         <v>0</v>
       </c>
       <c r="AR294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295">
@@ -46258,7 +46258,7 @@
         <v>0</v>
       </c>
       <c r="AR295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296">
@@ -46732,7 +46732,7 @@
         <v>0</v>
       </c>
       <c r="AR298" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299">
@@ -46763,7 +46763,7 @@
       <c r="I299" t="inlineStr"/>
       <c r="J299" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K299" t="inlineStr">
@@ -46917,7 +46917,7 @@
       </c>
       <c r="J300" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K300" t="inlineStr">
@@ -47030,7 +47030,7 @@
         <v>1</v>
       </c>
       <c r="AR300" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301">
@@ -47075,7 +47075,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K301" t="inlineStr">
@@ -47188,7 +47188,7 @@
         <v>1</v>
       </c>
       <c r="AR301" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302">
@@ -47233,7 +47233,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K302" t="inlineStr">
@@ -47346,7 +47346,7 @@
         <v>1</v>
       </c>
       <c r="AR302" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="303">
@@ -47391,7 +47391,7 @@
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K303" t="inlineStr">
@@ -47504,7 +47504,7 @@
         <v>1</v>
       </c>
       <c r="AR303" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="304">
@@ -47549,7 +47549,7 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K304" t="inlineStr">
@@ -47662,7 +47662,7 @@
         <v>1</v>
       </c>
       <c r="AR304" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305">
@@ -47707,7 +47707,7 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K305" t="inlineStr">
@@ -47865,7 +47865,7 @@
       </c>
       <c r="J306" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Japan']</t>
+          <t>['Japan', 'Netherlands']</t>
         </is>
       </c>
       <c r="K306" t="inlineStr">
@@ -48276,7 +48276,7 @@
         <v>0</v>
       </c>
       <c r="AR308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309">
@@ -48434,7 +48434,7 @@
         <v>0</v>
       </c>
       <c r="AR309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310">
@@ -48592,7 +48592,7 @@
         <v>0</v>
       </c>
       <c r="AR310" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="311">
@@ -48623,7 +48623,7 @@
       <c r="I311" t="inlineStr"/>
       <c r="J311" t="inlineStr">
         <is>
-          <t>['Chile', 'Spain']</t>
+          <t>['Spain', 'Chile']</t>
         </is>
       </c>
       <c r="K311" t="inlineStr">
@@ -48777,7 +48777,7 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>['Chile', 'Spain']</t>
+          <t>['Spain', 'Chile']</t>
         </is>
       </c>
       <c r="K312" t="inlineStr">
@@ -48890,7 +48890,7 @@
         <v>0</v>
       </c>
       <c r="AR312" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="313">
@@ -48935,7 +48935,7 @@
       </c>
       <c r="J313" t="inlineStr">
         <is>
-          <t>['Chile', 'Spain']</t>
+          <t>['Spain', 'Chile']</t>
         </is>
       </c>
       <c r="K313" t="inlineStr">
@@ -49048,7 +49048,7 @@
         <v>0</v>
       </c>
       <c r="AR313" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314">
@@ -49093,7 +49093,7 @@
       </c>
       <c r="J314" t="inlineStr">
         <is>
-          <t>['Chile', 'Spain']</t>
+          <t>['Spain', 'Chile']</t>
         </is>
       </c>
       <c r="K314" t="inlineStr">
@@ -49206,7 +49206,7 @@
         <v>0</v>
       </c>
       <c r="AR314" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315">
@@ -49504,7 +49504,7 @@
         <v>0</v>
       </c>
       <c r="AR316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317">
@@ -49662,7 +49662,7 @@
         <v>0</v>
       </c>
       <c r="AR317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318">
@@ -49820,7 +49820,7 @@
         <v>0</v>
       </c>
       <c r="AR318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319">
@@ -49978,7 +49978,7 @@
         <v>0</v>
       </c>
       <c r="AR319" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320">
@@ -50136,7 +50136,7 @@
         <v>0</v>
       </c>
       <c r="AR320" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321">
@@ -50167,7 +50167,7 @@
       <c r="I321" t="inlineStr"/>
       <c r="J321" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K321" t="inlineStr">
@@ -50321,7 +50321,7 @@
       </c>
       <c r="J322" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K322" t="inlineStr">
@@ -50434,7 +50434,7 @@
         <v>1</v>
       </c>
       <c r="AR322" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323">
@@ -50479,7 +50479,7 @@
       </c>
       <c r="J323" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K323" t="inlineStr">
@@ -50592,7 +50592,7 @@
         <v>1</v>
       </c>
       <c r="AR323" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324">
@@ -50637,7 +50637,7 @@
       </c>
       <c r="J324" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K324" t="inlineStr">
@@ -50795,7 +50795,7 @@
       </c>
       <c r="J325" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K325" t="inlineStr">
@@ -50953,7 +50953,7 @@
       </c>
       <c r="J326" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K326" t="inlineStr">
@@ -51066,7 +51066,7 @@
         <v>1</v>
       </c>
       <c r="AR326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="327">
@@ -51111,7 +51111,7 @@
       </c>
       <c r="J327" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K327" t="inlineStr">
@@ -51224,7 +51224,7 @@
         <v>1</v>
       </c>
       <c r="AR327" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328">
@@ -51269,7 +51269,7 @@
       </c>
       <c r="J328" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K328" t="inlineStr">
@@ -51427,7 +51427,7 @@
       </c>
       <c r="J329" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K329" t="inlineStr">
@@ -51540,7 +51540,7 @@
         <v>1</v>
       </c>
       <c r="AR329" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="330">
@@ -51585,7 +51585,7 @@
       </c>
       <c r="J330" t="inlineStr">
         <is>
-          <t>['Brazil', 'Mexico']</t>
+          <t>['Mexico', 'Brazil']</t>
         </is>
       </c>
       <c r="K330" t="inlineStr">
@@ -51698,7 +51698,7 @@
         <v>1</v>
       </c>
       <c r="AR330" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="331">
@@ -51996,7 +51996,7 @@
         <v>1</v>
       </c>
       <c r="AR332" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="333">
@@ -52294,7 +52294,7 @@
         <v>1</v>
       </c>
       <c r="AR334" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="335">
@@ -52339,7 +52339,7 @@
       </c>
       <c r="J335" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K335" t="inlineStr">
@@ -52452,7 +52452,7 @@
         <v>1</v>
       </c>
       <c r="AR335" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="336">
@@ -52497,7 +52497,7 @@
       </c>
       <c r="J336" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K336" t="inlineStr">
@@ -52655,7 +52655,7 @@
       </c>
       <c r="J337" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K337" t="inlineStr">
@@ -52926,7 +52926,7 @@
         <v>1</v>
       </c>
       <c r="AR338" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="339">
@@ -53287,7 +53287,7 @@
       </c>
       <c r="J341" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K341" t="inlineStr">
@@ -53431,7 +53431,7 @@
       <c r="I342" t="inlineStr"/>
       <c r="J342" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K342" t="inlineStr">
@@ -53585,7 +53585,7 @@
       </c>
       <c r="J343" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K343" t="inlineStr">
@@ -53698,7 +53698,7 @@
         <v>0</v>
       </c>
       <c r="AR343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344">
@@ -53743,7 +53743,7 @@
       </c>
       <c r="J344" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K344" t="inlineStr">
@@ -53856,7 +53856,7 @@
         <v>0</v>
       </c>
       <c r="AR344" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345">
@@ -53901,7 +53901,7 @@
       </c>
       <c r="J345" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K345" t="inlineStr">
@@ -54014,7 +54014,7 @@
         <v>0</v>
       </c>
       <c r="AR345" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="346">
@@ -54059,7 +54059,7 @@
       </c>
       <c r="J346" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K346" t="inlineStr">
@@ -54172,7 +54172,7 @@
         <v>0</v>
       </c>
       <c r="AR346" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="347">
@@ -54217,7 +54217,7 @@
       </c>
       <c r="J347" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K347" t="inlineStr">
@@ -54330,7 +54330,7 @@
         <v>0</v>
       </c>
       <c r="AR347" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="348">
@@ -54375,7 +54375,7 @@
       </c>
       <c r="J348" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K348" t="inlineStr">
@@ -54488,7 +54488,7 @@
         <v>0</v>
       </c>
       <c r="AR348" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="349">
@@ -54533,7 +54533,7 @@
       </c>
       <c r="J349" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K349" t="inlineStr">
@@ -54691,7 +54691,7 @@
       </c>
       <c r="J350" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K350" t="inlineStr">
@@ -54804,7 +54804,7 @@
         <v>0</v>
       </c>
       <c r="AR350" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="351">
@@ -54849,7 +54849,7 @@
       </c>
       <c r="J351" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K351" t="inlineStr">
@@ -54962,7 +54962,7 @@
         <v>0</v>
       </c>
       <c r="AR351" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="352">
@@ -55260,7 +55260,7 @@
         <v>0</v>
       </c>
       <c r="AR353" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="354">
@@ -55418,7 +55418,7 @@
         <v>0</v>
       </c>
       <c r="AR354" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355">
@@ -55576,7 +55576,7 @@
         <v>0</v>
       </c>
       <c r="AR355" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="356">
@@ -55607,7 +55607,7 @@
       <c r="I356" t="inlineStr"/>
       <c r="J356" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K356" t="inlineStr">
@@ -55761,7 +55761,7 @@
       </c>
       <c r="J357" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K357" t="inlineStr">
@@ -55874,7 +55874,7 @@
         <v>0</v>
       </c>
       <c r="AR357" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="358">
@@ -55919,7 +55919,7 @@
       </c>
       <c r="J358" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K358" t="inlineStr">
@@ -56032,7 +56032,7 @@
         <v>0</v>
       </c>
       <c r="AR358" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="359">
@@ -56077,7 +56077,7 @@
       </c>
       <c r="J359" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K359" t="inlineStr">
@@ -56235,7 +56235,7 @@
       </c>
       <c r="J360" t="inlineStr">
         <is>
-          <t>['Germany', 'United States']</t>
+          <t>['United States', 'Germany']</t>
         </is>
       </c>
       <c r="K360" t="inlineStr">
@@ -56348,7 +56348,7 @@
         <v>0</v>
       </c>
       <c r="AR360" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="361">
@@ -56646,7 +56646,7 @@
         <v>1</v>
       </c>
       <c r="AR362" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="363">
@@ -56804,7 +56804,7 @@
         <v>1</v>
       </c>
       <c r="AR363" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="364">
@@ -57147,7 +57147,7 @@
       </c>
       <c r="J366" t="inlineStr">
         <is>
-          <t>['Russia', 'Uruguay']</t>
+          <t>['Uruguay', 'Russia']</t>
         </is>
       </c>
       <c r="K366" t="inlineStr">
@@ -57260,7 +57260,7 @@
         <v>0</v>
       </c>
       <c r="AR366" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367">
@@ -57305,7 +57305,7 @@
       </c>
       <c r="J367" t="inlineStr">
         <is>
-          <t>['Russia', 'Uruguay']</t>
+          <t>['Uruguay', 'Russia']</t>
         </is>
       </c>
       <c r="K367" t="inlineStr">
@@ -57418,7 +57418,7 @@
         <v>0</v>
       </c>
       <c r="AR367" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368">
@@ -57463,7 +57463,7 @@
       </c>
       <c r="J368" t="inlineStr">
         <is>
-          <t>['Russia', 'Uruguay']</t>
+          <t>['Uruguay', 'Russia']</t>
         </is>
       </c>
       <c r="K368" t="inlineStr">
@@ -57576,7 +57576,7 @@
         <v>0</v>
       </c>
       <c r="AR368" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="369">
@@ -57621,7 +57621,7 @@
       </c>
       <c r="J369" t="inlineStr">
         <is>
-          <t>['Russia', 'Uruguay']</t>
+          <t>['Uruguay', 'Russia']</t>
         </is>
       </c>
       <c r="K369" t="inlineStr">
@@ -57734,7 +57734,7 @@
         <v>0</v>
       </c>
       <c r="AR369" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="370">
@@ -57779,7 +57779,7 @@
       </c>
       <c r="J370" t="inlineStr">
         <is>
-          <t>['Russia', 'Uruguay']</t>
+          <t>['Uruguay', 'Russia']</t>
         </is>
       </c>
       <c r="K370" t="inlineStr">
@@ -57892,7 +57892,7 @@
         <v>0</v>
       </c>
       <c r="AR370" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="371">
@@ -57937,7 +57937,7 @@
       </c>
       <c r="J371" t="inlineStr">
         <is>
-          <t>['Russia', 'Uruguay']</t>
+          <t>['Uruguay', 'Russia']</t>
         </is>
       </c>
       <c r="K371" t="inlineStr">
@@ -58050,7 +58050,7 @@
         <v>0</v>
       </c>
       <c r="AR371" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="372">
@@ -58081,7 +58081,7 @@
       <c r="I372" t="inlineStr"/>
       <c r="J372" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K372" t="inlineStr">
@@ -58235,7 +58235,7 @@
       </c>
       <c r="J373" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K373" t="inlineStr">
@@ -58348,7 +58348,7 @@
         <v>0</v>
       </c>
       <c r="AR373" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374">
@@ -58393,7 +58393,7 @@
       </c>
       <c r="J374" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K374" t="inlineStr">
@@ -58506,7 +58506,7 @@
         <v>1</v>
       </c>
       <c r="AR374" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375">
@@ -58551,7 +58551,7 @@
       </c>
       <c r="J375" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K375" t="inlineStr">
@@ -58664,7 +58664,7 @@
         <v>0</v>
       </c>
       <c r="AR375" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="376">
@@ -58709,7 +58709,7 @@
       </c>
       <c r="J376" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K376" t="inlineStr">
@@ -58822,7 +58822,7 @@
         <v>1</v>
       </c>
       <c r="AR376" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377">
@@ -58867,7 +58867,7 @@
       </c>
       <c r="J377" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K377" t="inlineStr">
@@ -58980,7 +58980,7 @@
         <v>0</v>
       </c>
       <c r="AR377" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="378">
@@ -59025,7 +59025,7 @@
       </c>
       <c r="J378" t="inlineStr">
         <is>
-          <t>['Portugal', 'Spain']</t>
+          <t>['Spain', 'Portugal']</t>
         </is>
       </c>
       <c r="K378" t="inlineStr">
@@ -59436,7 +59436,7 @@
         <v>0</v>
       </c>
       <c r="AR380" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381">
@@ -59594,7 +59594,7 @@
         <v>0</v>
       </c>
       <c r="AR381" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382">
@@ -59892,7 +59892,7 @@
         <v>1</v>
       </c>
       <c r="AR383" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384">
@@ -60050,7 +60050,7 @@
         <v>0</v>
       </c>
       <c r="AR384" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385">
@@ -60366,7 +60366,7 @@
         <v>0</v>
       </c>
       <c r="AR386" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="387">
@@ -60524,7 +60524,7 @@
         <v>1</v>
       </c>
       <c r="AR387" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="388">
@@ -60980,7 +60980,7 @@
         <v>0</v>
       </c>
       <c r="AR390" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391">
@@ -61138,7 +61138,7 @@
         <v>0</v>
       </c>
       <c r="AR391" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392">
@@ -61454,7 +61454,7 @@
         <v>0</v>
       </c>
       <c r="AR393" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394">
@@ -61612,7 +61612,7 @@
         <v>0</v>
       </c>
       <c r="AR394" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395">
@@ -61910,7 +61910,7 @@
         <v>1</v>
       </c>
       <c r="AR396" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="397">
@@ -62068,7 +62068,7 @@
         <v>0</v>
       </c>
       <c r="AR397" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="398">
@@ -62226,7 +62226,7 @@
         <v>0</v>
       </c>
       <c r="AR398" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="399">
@@ -62384,7 +62384,7 @@
         <v>0</v>
       </c>
       <c r="AR399" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400">
@@ -62542,7 +62542,7 @@
         <v>0</v>
       </c>
       <c r="AR400" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="401">
@@ -62700,7 +62700,7 @@
         <v>0</v>
       </c>
       <c r="AR401" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="402">
@@ -62731,7 +62731,7 @@
       <c r="I402" t="inlineStr"/>
       <c r="J402" t="inlineStr">
         <is>
-          <t>['Senegal', 'Japan']</t>
+          <t>['Japan', 'Senegal']</t>
         </is>
       </c>
       <c r="K402" t="inlineStr">
@@ -62885,7 +62885,7 @@
       </c>
       <c r="J403" t="inlineStr">
         <is>
-          <t>['Senegal', 'Colombia']</t>
+          <t>['Colombia', 'Senegal']</t>
         </is>
       </c>
       <c r="K403" t="inlineStr">
@@ -62998,7 +62998,7 @@
         <v>0</v>
       </c>
       <c r="AR403" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="404">
@@ -63043,7 +63043,7 @@
       </c>
       <c r="J404" t="inlineStr">
         <is>
-          <t>['Senegal', 'Colombia']</t>
+          <t>['Colombia', 'Senegal']</t>
         </is>
       </c>
       <c r="K404" t="inlineStr">
@@ -63156,7 +63156,7 @@
         <v>0</v>
       </c>
       <c r="AR404" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="405">
@@ -63454,7 +63454,7 @@
         <v>0</v>
       </c>
       <c r="AR406" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="407">
@@ -63612,7 +63612,7 @@
         <v>0</v>
       </c>
       <c r="AR407" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="408">
@@ -63770,7 +63770,7 @@
         <v>0</v>
       </c>
       <c r="AR408" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="409">
@@ -63928,7 +63928,7 @@
         <v>0</v>
       </c>
       <c r="AR409" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="410">
@@ -64226,7 +64226,7 @@
         <v>1</v>
       </c>
       <c r="AR411" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="412">
@@ -64384,7 +64384,7 @@
         <v>1</v>
       </c>
       <c r="AR412" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="413">
@@ -64858,7 +64858,7 @@
         <v>1</v>
       </c>
       <c r="AR415" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="416">
@@ -64889,7 +64889,7 @@
       <c r="I416" t="inlineStr"/>
       <c r="J416" t="inlineStr">
         <is>
-          <t>['England', 'Iran']</t>
+          <t>['Iran', 'England']</t>
         </is>
       </c>
       <c r="K416" t="inlineStr">
@@ -65156,7 +65156,7 @@
         <v>1</v>
       </c>
       <c r="AR417" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="418">
@@ -65314,7 +65314,7 @@
         <v>1</v>
       </c>
       <c r="AR418" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="419">
@@ -65661,7 +65661,7 @@
       <c r="I421" t="inlineStr"/>
       <c r="J421" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K421" t="inlineStr">
@@ -65928,7 +65928,7 @@
         <v>0</v>
       </c>
       <c r="AR422" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423">
@@ -65973,7 +65973,7 @@
       </c>
       <c r="J423" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K423" t="inlineStr">
@@ -66086,7 +66086,7 @@
         <v>0</v>
       </c>
       <c r="AR423" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="424">
@@ -66384,7 +66384,7 @@
         <v>0</v>
       </c>
       <c r="AR425" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="426">
@@ -66542,7 +66542,7 @@
         <v>0</v>
       </c>
       <c r="AR426" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="427">
@@ -66858,7 +66858,7 @@
         <v>0</v>
       </c>
       <c r="AR428" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="429">
@@ -67016,7 +67016,7 @@
         <v>0</v>
       </c>
       <c r="AR429" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430">
@@ -67314,7 +67314,7 @@
         <v>1</v>
       </c>
       <c r="AR431" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432">
@@ -67472,7 +67472,7 @@
         <v>1</v>
       </c>
       <c r="AR432" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="433">
@@ -67815,7 +67815,7 @@
       </c>
       <c r="J435" t="inlineStr">
         <is>
-          <t>['Germany', 'Spain']</t>
+          <t>['Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K435" t="inlineStr">
@@ -67928,7 +67928,7 @@
         <v>0</v>
       </c>
       <c r="AR435" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436">
@@ -67973,7 +67973,7 @@
       </c>
       <c r="J436" t="inlineStr">
         <is>
-          <t>['Germany', 'Spain']</t>
+          <t>['Spain', 'Germany']</t>
         </is>
       </c>
       <c r="K436" t="inlineStr">
@@ -68086,7 +68086,7 @@
         <v>0</v>
       </c>
       <c r="AR436" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="437">
@@ -68244,7 +68244,7 @@
         <v>0</v>
       </c>
       <c r="AR437" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="438">
@@ -68289,7 +68289,7 @@
       </c>
       <c r="J438" t="inlineStr">
         <is>
-          <t>['Spain', 'Japan']</t>
+          <t>['Japan', 'Spain']</t>
         </is>
       </c>
       <c r="K438" t="inlineStr">
@@ -68402,7 +68402,7 @@
         <v>0</v>
       </c>
       <c r="AR438" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439">
@@ -68447,7 +68447,7 @@
       </c>
       <c r="J439" t="inlineStr">
         <is>
-          <t>['Spain', 'Japan']</t>
+          <t>['Japan', 'Spain']</t>
         </is>
       </c>
       <c r="K439" t="inlineStr">
@@ -68560,7 +68560,7 @@
         <v>0</v>
       </c>
       <c r="AR439" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440">
@@ -68718,7 +68718,7 @@
         <v>0</v>
       </c>
       <c r="AR440" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441">
@@ -68763,7 +68763,7 @@
       </c>
       <c r="J441" t="inlineStr">
         <is>
-          <t>['Spain', 'Japan']</t>
+          <t>['Japan', 'Spain']</t>
         </is>
       </c>
       <c r="K441" t="inlineStr">
@@ -68921,7 +68921,7 @@
       </c>
       <c r="J442" t="inlineStr">
         <is>
-          <t>['Spain', 'Japan']</t>
+          <t>['Japan', 'Spain']</t>
         </is>
       </c>
       <c r="K442" t="inlineStr">
@@ -69034,7 +69034,7 @@
         <v>0</v>
       </c>
       <c r="AR442" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="443">
@@ -69079,7 +69079,7 @@
       </c>
       <c r="J443" t="inlineStr">
         <is>
-          <t>['Spain', 'Japan']</t>
+          <t>['Japan', 'Spain']</t>
         </is>
       </c>
       <c r="K443" t="inlineStr">
@@ -69192,7 +69192,7 @@
         <v>0</v>
       </c>
       <c r="AR443" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444">
@@ -69223,7 +69223,7 @@
       <c r="I444" t="inlineStr"/>
       <c r="J444" t="inlineStr">
         <is>
-          <t>['Portugal', 'Ghana']</t>
+          <t>['Ghana', 'Portugal']</t>
         </is>
       </c>
       <c r="K444" t="inlineStr">
@@ -69377,7 +69377,7 @@
       </c>
       <c r="J445" t="inlineStr">
         <is>
-          <t>['Portugal', 'Ghana']</t>
+          <t>['Ghana', 'Portugal']</t>
         </is>
       </c>
       <c r="K445" t="inlineStr">
@@ -69490,7 +69490,7 @@
         <v>1</v>
       </c>
       <c r="AR445" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="446">
@@ -69535,7 +69535,7 @@
       </c>
       <c r="J446" t="inlineStr">
         <is>
-          <t>['Portugal', 'Uruguay']</t>
+          <t>['Uruguay', 'Portugal']</t>
         </is>
       </c>
       <c r="K446" t="inlineStr">
@@ -69648,7 +69648,7 @@
         <v>1</v>
       </c>
       <c r="AR446" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="447">
@@ -69693,7 +69693,7 @@
       </c>
       <c r="J447" t="inlineStr">
         <is>
-          <t>['Portugal', 'Uruguay']</t>
+          <t>['Uruguay', 'Portugal']</t>
         </is>
       </c>
       <c r="K447" t="inlineStr">
@@ -69851,7 +69851,7 @@
       </c>
       <c r="J448" t="inlineStr">
         <is>
-          <t>['Portugal', 'Uruguay']</t>
+          <t>['Uruguay', 'Portugal']</t>
         </is>
       </c>
       <c r="K448" t="inlineStr">
@@ -69964,7 +69964,7 @@
         <v>1</v>
       </c>
       <c r="AR448" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="449">
@@ -70009,7 +70009,7 @@
       </c>
       <c r="J449" t="inlineStr">
         <is>
-          <t>['Portugal', 'South Korea']</t>
+          <t>['South Korea', 'Portugal']</t>
         </is>
       </c>
       <c r="K449" t="inlineStr">
@@ -70122,7 +70122,7 @@
         <v>0</v>
       </c>
       <c r="AR449" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450">
@@ -70420,7 +70420,7 @@
         <v>0</v>
       </c>
       <c r="AR451" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="452">
@@ -70578,7 +70578,7 @@
         <v>0</v>
       </c>
       <c r="AR452" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="453">
@@ -71052,7 +71052,7 @@
         <v>0</v>
       </c>
       <c r="AR455" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="456">
@@ -71210,7 +71210,7 @@
         <v>0</v>
       </c>
       <c r="AR456" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>